<commit_message>
update plasmid construction template
</commit_message>
<xml_diff>
--- a/templates/community/CEPLAS-data/plasmid_construction.xlsx
+++ b/templates/community/CEPLAS-data/plasmid_construction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t_ori\Desktop\arcs\Swate-templates\templates\community\CEPLAS-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48D9A5EB-E02F-481A-8777-DD3288185BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56E50CF-3EE3-4C0B-9725-912942ECEEED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="1" xr2:uid="{69ECA3DE-E052-492B-A55E-C3A7BB6843BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{69ECA3DE-E052-492B-A55E-C3A7BB6843BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
   <si>
     <t>Id</t>
   </si>
@@ -197,6 +197,24 @@
   </si>
   <si>
     <t>ENVO</t>
+  </si>
+  <si>
+    <t>Parameter [tag]</t>
+  </si>
+  <si>
+    <t>Term Source REF (MI:0507)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (MI:0507)</t>
+  </si>
+  <si>
+    <t>Parameter [terminator]</t>
+  </si>
+  <si>
+    <t>Term Source REF (SO:0000141)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (SO:0000141)</t>
   </si>
 </sst>
 </file>
@@ -381,7 +399,25 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="15">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -423,19 +459,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4D48BF83-1766-47EE-B342-D64615C087EB}" name="annotationTableChattyQuail35" displayName="annotationTableChattyQuail35" ref="A1:K2" totalsRowShown="0">
-  <autoFilter ref="A1:K2" xr:uid="{4D48BF83-1766-47EE-B342-D64615C087EB}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4D48BF83-1766-47EE-B342-D64615C087EB}" name="annotationTableChattyQuail35" displayName="annotationTableChattyQuail35" ref="A1:Q2" totalsRowShown="0">
+  <autoFilter ref="A1:Q2" xr:uid="{4D48BF83-1766-47EE-B342-D64615C087EB}"/>
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{E53B771E-B8D6-4DD6-9FE0-67403378F947}" name="Source Name"/>
-    <tableColumn id="3" xr3:uid="{2EFE6B4C-CFC9-43E1-81C3-2AF59D0F49B1}" name="Characteristic [Promoter]" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{A3C48F52-5A9E-419D-81CD-0543FA1CD52E}" name="Term Source REF (NCIT:C13297)" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{2AD1F491-1A9B-4E9A-8529-6855688C3DD5}" name="Term Accession Number (NCIT:C13297)" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{8C736FC3-58AC-49BC-8F8A-31BC08161D2C}" name="Characteristic [gene]" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{44AEE78F-B0AD-44F4-AC07-CA33418FB35E}" name="Term Source REF (SO:0000704)" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{5327E4FE-63E3-43DA-9F3C-E702F07BAA4C}" name="Term Accession Number (SO:0000704)" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{8534A25E-AB2B-49A1-ABBE-432C0C5CE3D1}" name="Characteristic [Antibiotic Resistance]" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{441C4D3F-1931-4502-9E8D-FB442AA5C475}" name="Term Source REF (NCIT:C17449)" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{EC33F04D-306E-431D-9BA7-BDF1DE2B7879}" name="Term Accession Number (NCIT:C17449)" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{2EFE6B4C-CFC9-43E1-81C3-2AF59D0F49B1}" name="Characteristic [Promoter]" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{A3C48F52-5A9E-419D-81CD-0543FA1CD52E}" name="Term Source REF (NCIT:C13297)" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{2AD1F491-1A9B-4E9A-8529-6855688C3DD5}" name="Term Accession Number (NCIT:C13297)" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{8C736FC3-58AC-49BC-8F8A-31BC08161D2C}" name="Characteristic [gene]" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{44AEE78F-B0AD-44F4-AC07-CA33418FB35E}" name="Term Source REF (SO:0000704)" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{5327E4FE-63E3-43DA-9F3C-E702F07BAA4C}" name="Term Accession Number (SO:0000704)" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{8534A25E-AB2B-49A1-ABBE-432C0C5CE3D1}" name="Characteristic [Antibiotic Resistance]" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{441C4D3F-1931-4502-9E8D-FB442AA5C475}" name="Term Source REF (NCIT:C17449)" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{EC33F04D-306E-431D-9BA7-BDF1DE2B7879}" name="Term Accession Number (NCIT:C17449)" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{99F0DD35-51D8-440B-8B5E-710F05E26B22}" name="Parameter [tag]" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{54189832-0DA3-49D0-A7A3-E0B2FC840B14}" name="Term Source REF (MI:0507)" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{C0D5FB71-F04B-422A-8BA1-E1C7A3C48C01}" name="Term Accession Number (MI:0507)" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{B5109C2E-C49E-4AA9-9620-4ED47BCD87A2}" name="Parameter [terminator]" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{63D05357-388E-4B9A-8B10-381047362851}" name="Term Source REF (SO:0000141)" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{44869EAD-4F1A-462C-BD73-FE737E45A3EF}" name="Term Accession Number (SO:0000141)" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{D4307DB3-C401-448B-88FC-16BF964AAD34}" name="Sample Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -742,7 +784,7 @@
   <wetp:taskpane dockstate="right" visibility="0" width="438" row="0">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
-  <wetp:taskpane dockstate="right" visibility="0" width="473" row="1">
+  <wetp:taskpane dockstate="right" visibility="0" width="574" row="0">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -770,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E67034-0761-4AA3-A7BB-D4E5F5D732CB}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -788,10 +830,16 @@
     <col min="8" max="8" width="34.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.109375" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="36.6640625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.21875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="32.77734375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.33203125" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="35.88671875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -823,10 +871,28 @@
         <v>43</v>
       </c>
       <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
         <v>35</v>
@@ -850,6 +916,24 @@
         <v>35</v>
       </c>
       <c r="J2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="10" t="s">
         <v>35</v>
       </c>
     </row>
@@ -865,7 +949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30C783F3-B0A1-4DEF-A92E-1D7E3EFD83D4}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>